<commit_message>
Nuevos Casos de Uso 20-09-2012
</commit_message>
<xml_diff>
--- a/Tareas Juan.xlsx
+++ b/Tareas Juan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
   <si>
     <t>CU-034</t>
   </si>
@@ -82,6 +82,72 @@
   </si>
   <si>
     <t>9:30pm</t>
+  </si>
+  <si>
+    <t>TAREA</t>
+  </si>
+  <si>
+    <t>FECHA</t>
+  </si>
+  <si>
+    <t>HORA</t>
+  </si>
+  <si>
+    <t>CU-033 Aceptar peticion de conexion</t>
+  </si>
+  <si>
+    <t>CU-034 Aceptar peticion de desconexion</t>
+  </si>
+  <si>
+    <t>CU-035 Añadir  jugador a sala</t>
+  </si>
+  <si>
+    <t>CU-036 Retornar informacion de salas de juego</t>
+  </si>
+  <si>
+    <t>CU-037 Iniciar emulación del Juego</t>
+  </si>
+  <si>
+    <t>CU-041 Eliminar jugador de sala de juego</t>
+  </si>
+  <si>
+    <t>Control y Evaluación del Proyecto</t>
+  </si>
+  <si>
+    <t>Plan de Metricas</t>
+  </si>
+  <si>
+    <t>Plan de Gestion de Calidad</t>
+  </si>
+  <si>
+    <t>CU-042 Retornar resultado del juego</t>
+  </si>
+  <si>
+    <t>CU-043 Eliminar jugador de Simulacion</t>
+  </si>
+  <si>
+    <t>11:00am</t>
+  </si>
+  <si>
+    <t>9:55am</t>
+  </si>
+  <si>
+    <t>11:20pm</t>
+  </si>
+  <si>
+    <t>9:35am</t>
+  </si>
+  <si>
+    <t>10:10am</t>
+  </si>
+  <si>
+    <t>9:00am</t>
+  </si>
+  <si>
+    <t>9:25am</t>
+  </si>
+  <si>
+    <t>10:35am</t>
   </si>
 </sst>
 </file>
@@ -117,7 +183,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -141,40 +207,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -461,6 +497,178 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -469,53 +677,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,225 +1051,481 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="1" max="1" width="44" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="48.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="32" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="8">
         <v>41171</v>
       </c>
-      <c r="C2" s="8">
-        <v>0.875</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="27">
+      <c r="C2" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="24">
         <v>41168</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="9">
         <v>41171</v>
       </c>
-      <c r="C3" s="9">
-        <v>0.875</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="26">
+      <c r="C3" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="23">
         <v>41168</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="9">
         <v>41171</v>
       </c>
-      <c r="C4" s="9">
-        <v>0.875</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="26">
+      <c r="C4" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="23">
         <v>41168</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="9">
         <v>41171</v>
       </c>
-      <c r="C5" s="9">
-        <v>0.875</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="26">
+      <c r="C5" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="23">
         <v>41168</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="9">
         <v>41171</v>
       </c>
-      <c r="C6" s="9">
-        <v>0.875</v>
-      </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="26">
+      <c r="C6" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="23">
         <v>41169</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="9">
         <v>41171</v>
       </c>
-      <c r="C7" s="9">
-        <v>0.875</v>
-      </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="26">
+      <c r="C7" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="23">
         <v>41169</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="9">
         <v>41171</v>
       </c>
-      <c r="C8" s="9">
-        <v>0.875</v>
-      </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="26">
+      <c r="C8" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="23">
         <v>41170</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="10">
         <v>41171</v>
       </c>
-      <c r="C9" s="10">
-        <v>0.875</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="11">
+      <c r="C9" s="7">
+        <v>0.875</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="39">
         <v>41171</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="3" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="8">
+        <v>41172</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="D11" s="33"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="24">
+        <v>41172</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="9">
+        <v>41172</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="23">
+        <v>41172</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="9">
+        <v>41172</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="23">
+        <v>41172</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
+      <c r="A14" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="9">
+        <v>41172</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D14" s="34"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="23">
+        <v>41172</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="9">
+        <v>41172</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D15" s="34"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="23">
+        <v>41172</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="9">
+        <v>41172</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="23">
+        <v>41172</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="9">
+        <v>41172</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D17" s="34"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="23">
+        <v>41172</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="9">
+        <v>41172</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D18" s="35"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="23">
+        <v>41172</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="9">
+        <v>41173</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="27"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="9">
+        <v>41173</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="27"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="10">
+        <v>41173</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0.875</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="21"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
V&V de Casos de Uso
</commit_message>
<xml_diff>
--- a/Tareas Juan.xlsx
+++ b/Tareas Juan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
     <t>CU-034</t>
   </si>
@@ -126,28 +126,40 @@
     <t>CU-043 Eliminar jugador de Simulacion</t>
   </si>
   <si>
-    <t>11:00am</t>
-  </si>
-  <si>
-    <t>9:55am</t>
-  </si>
-  <si>
-    <t>11:20pm</t>
-  </si>
-  <si>
-    <t>9:35am</t>
-  </si>
-  <si>
-    <t>10:10am</t>
-  </si>
-  <si>
-    <t>9:00am</t>
-  </si>
-  <si>
-    <t>9:25am</t>
-  </si>
-  <si>
-    <t>10:35am</t>
+    <t>Planes</t>
+  </si>
+  <si>
+    <t>Puntos caso de Uso</t>
+  </si>
+  <si>
+    <t>SPMP Vision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRS Linea base </t>
+  </si>
+  <si>
+    <t>V&amp;V CU-001 Conectar al servidor</t>
+  </si>
+  <si>
+    <t>V&amp;V CU-002 Desconectar del servidor</t>
+  </si>
+  <si>
+    <t>V&amp;V CU-010 Abandonar simulacion</t>
+  </si>
+  <si>
+    <t>V&amp;V CU-011 Salir del juego</t>
+  </si>
+  <si>
+    <t>V&amp;V CU-012 Salir de sala de juego</t>
+  </si>
+  <si>
+    <t>V&amp;V CU-020 ver cartas de juego</t>
+  </si>
+  <si>
+    <t>V&amp;V CU-021 ver reglas del juego</t>
+  </si>
+  <si>
+    <t>V&amp;V CU-023 ver ayuda del juego</t>
   </si>
 </sst>
 </file>
@@ -183,7 +195,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -530,17 +542,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -673,11 +674,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -722,34 +745,40 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1051,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,13 +1102,13 @@
       <c r="A1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -1088,10 +1117,10 @@
       <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="31" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1264,7 +1293,7 @@
       <c r="F9" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="39">
+      <c r="G9" s="38">
         <v>41171</v>
       </c>
       <c r="H9" s="3" t="s">
@@ -1275,13 +1304,13 @@
       <c r="A10" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="39" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -1290,15 +1319,15 @@
       <c r="F10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="G10" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="32" t="s">
+      <c r="H10" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="36" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="8">
@@ -1307,7 +1336,7 @@
       <c r="C11" s="5">
         <v>0.875</v>
       </c>
-      <c r="D11" s="33"/>
+      <c r="D11" s="32"/>
       <c r="E11" s="17"/>
       <c r="F11" s="18" t="s">
         <v>15</v>
@@ -1315,12 +1344,12 @@
       <c r="G11" s="24">
         <v>41172</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>41</v>
+      <c r="H11" s="46">
+        <v>0.375</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="37" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="9">
@@ -1329,7 +1358,7 @@
       <c r="C12" s="6">
         <v>0.875</v>
       </c>
-      <c r="D12" s="34"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="19"/>
       <c r="F12" s="20" t="s">
         <v>15</v>
@@ -1337,12 +1366,12 @@
       <c r="G12" s="23">
         <v>41172</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>42</v>
+      <c r="H12" s="47">
+        <v>0.3923611111111111</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="37" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="9">
@@ -1351,7 +1380,7 @@
       <c r="C13" s="6">
         <v>0.875</v>
       </c>
-      <c r="D13" s="34"/>
+      <c r="D13" s="33"/>
       <c r="E13" s="19"/>
       <c r="F13" s="20" t="s">
         <v>15</v>
@@ -1359,12 +1388,12 @@
       <c r="G13" s="23">
         <v>41172</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>36</v>
+      <c r="H13" s="47">
+        <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="37" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="9">
@@ -1373,7 +1402,7 @@
       <c r="C14" s="6">
         <v>0.875</v>
       </c>
-      <c r="D14" s="34"/>
+      <c r="D14" s="33"/>
       <c r="E14" s="19"/>
       <c r="F14" s="20" t="s">
         <v>15</v>
@@ -1381,12 +1410,12 @@
       <c r="G14" s="23">
         <v>41172</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>37</v>
+      <c r="H14" s="47">
+        <v>0.41319444444444442</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="37" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="9">
@@ -1395,7 +1424,7 @@
       <c r="C15" s="6">
         <v>0.875</v>
       </c>
-      <c r="D15" s="34"/>
+      <c r="D15" s="33"/>
       <c r="E15" s="19"/>
       <c r="F15" s="20" t="s">
         <v>15</v>
@@ -1403,8 +1432,8 @@
       <c r="G15" s="23">
         <v>41172</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>40</v>
+      <c r="H15" s="47">
+        <v>0.4236111111111111</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1417,7 +1446,7 @@
       <c r="C16" s="6">
         <v>0.875</v>
       </c>
-      <c r="D16" s="34"/>
+      <c r="D16" s="33"/>
       <c r="E16" s="19"/>
       <c r="F16" s="20" t="s">
         <v>15</v>
@@ -1425,8 +1454,8 @@
       <c r="G16" s="23">
         <v>41172</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>43</v>
+      <c r="H16" s="47">
+        <v>0.44097222222222227</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1439,7 +1468,7 @@
       <c r="C17" s="6">
         <v>0.875</v>
       </c>
-      <c r="D17" s="34"/>
+      <c r="D17" s="33"/>
       <c r="E17" s="19"/>
       <c r="F17" s="20" t="s">
         <v>15</v>
@@ -1447,8 +1476,8 @@
       <c r="G17" s="23">
         <v>41172</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>39</v>
+      <c r="H17" s="47">
+        <v>0.39930555555555558</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1461,16 +1490,16 @@
       <c r="C18" s="6">
         <v>0.875</v>
       </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="28" t="s">
+      <c r="D18" s="34"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="27" t="s">
         <v>15</v>
       </c>
       <c r="G18" s="23">
         <v>41172</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>38</v>
+      <c r="H18" s="47">
+        <v>0.47222222222222227</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1483,13 +1512,17 @@
       <c r="C19" s="6">
         <v>0.875</v>
       </c>
-      <c r="D19" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="2"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="23">
+        <v>41173</v>
+      </c>
+      <c r="H19" s="47">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
@@ -1501,31 +1534,247 @@
       <c r="C20" s="6">
         <v>0.875</v>
       </c>
-      <c r="D20" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="29"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="42">
         <v>41173</v>
       </c>
       <c r="C21" s="7">
         <v>0.875</v>
       </c>
-      <c r="D21" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="21"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="F21" s="22"/>
-      <c r="G21" s="30"/>
+      <c r="G21" s="29"/>
       <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="8">
+        <v>41176</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="17"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="46"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="9">
+        <v>41180</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="47"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="9">
+        <v>41180</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="19"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="47"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="9">
+        <v>41180</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="19"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C26" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D26" s="33"/>
+      <c r="E26" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="20"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D27" s="33"/>
+      <c r="E27" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="20"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D28" s="34"/>
+      <c r="E28" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="27"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="D29" s="34"/>
+      <c r="E29" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="27"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="D30" s="34"/>
+      <c r="E30" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="27"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C31" s="6">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="D31" s="34"/>
+      <c r="E31" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="27"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="D32" s="34"/>
+      <c r="E32" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="27"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="10">
+        <v>41176</v>
+      </c>
+      <c r="C33" s="7">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D33" s="35"/>
+      <c r="E33" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="22"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Casos de uso refinamiento
</commit_message>
<xml_diff>
--- a/Tareas Juan.xlsx
+++ b/Tareas Juan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="18780" windowHeight="8580"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="18780" windowHeight="8580"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="65">
   <si>
     <t>CU-034</t>
   </si>
@@ -160,6 +160,57 @@
   </si>
   <si>
     <t>V&amp;V CU-023 ver ayuda del juego</t>
+  </si>
+  <si>
+    <t>Juan Pablo</t>
+  </si>
+  <si>
+    <t>CU-038 Asignar estado inicial del juego</t>
+  </si>
+  <si>
+    <t>CU-039 Asignar cartas de juego</t>
+  </si>
+  <si>
+    <t>CU-040 Asignar turno</t>
+  </si>
+  <si>
+    <t>CU-043 Eliminar jugador del Emulador</t>
+  </si>
+  <si>
+    <t>CU-046 Emular lanzamiento de dados</t>
+  </si>
+  <si>
+    <t>CU-050 Detener servicios</t>
+  </si>
+  <si>
+    <t>CU-051 Detener conexiones</t>
+  </si>
+  <si>
+    <t>CU-052 Guardar log de Sesion</t>
+  </si>
+  <si>
+    <t>CU-059 Procesar Sugerencia</t>
+  </si>
+  <si>
+    <t>CU-060 Mover Arma</t>
+  </si>
+  <si>
+    <t>CU-061 Mover Personaje Hacia Habitacion</t>
+  </si>
+  <si>
+    <t>CU-062 Informar Sugerencia a Jugadores</t>
+  </si>
+  <si>
+    <t>CU-064 Adicionar Sala de Juego</t>
+  </si>
+  <si>
+    <t>CU-065 Verificar Acusación</t>
+  </si>
+  <si>
+    <t>CU-066 Actualizar Tablero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CU-068 Finalizar Emulador </t>
   </si>
 </sst>
 </file>
@@ -175,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,8 +245,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="38">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -696,11 +753,72 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -779,6 +897,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1080,22 +1210,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="48.28515625" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" customWidth="1"/>
+    <col min="9" max="9" width="48.33203125" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" customWidth="1"/>
+    <col min="16" max="16" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1124,7 +1254,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
@@ -1146,7 +1276,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
@@ -1168,7 +1298,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
@@ -1190,7 +1320,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>0</v>
       </c>
@@ -1212,7 +1342,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>4</v>
       </c>
@@ -1234,7 +1364,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>5</v>
       </c>
@@ -1256,7 +1386,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>6</v>
       </c>
@@ -1326,7 +1456,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>25</v>
       </c>
@@ -1348,7 +1478,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="37" t="s">
         <v>26</v>
       </c>
@@ -1370,7 +1500,7 @@
         <v>0.3923611111111111</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
         <v>27</v>
       </c>
@@ -1392,7 +1522,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
         <v>28</v>
       </c>
@@ -1414,7 +1544,7 @@
         <v>0.41319444444444442</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="37" t="s">
         <v>29</v>
       </c>
@@ -1436,7 +1566,7 @@
         <v>0.4236111111111111</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>30</v>
       </c>
@@ -1458,7 +1588,7 @@
         <v>0.44097222222222227</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>34</v>
       </c>
@@ -1480,7 +1610,7 @@
         <v>0.39930555555555558</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>35</v>
       </c>
@@ -1502,7 +1632,7 @@
         <v>0.47222222222222227</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>31</v>
       </c>
@@ -1524,7 +1654,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>32</v>
       </c>
@@ -1535,10 +1665,10 @@
         <v>0.875</v>
       </c>
       <c r="D20" s="34"/>
-      <c r="E20" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="27"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="G20" s="28"/>
       <c r="H20" s="2"/>
     </row>
@@ -1553,14 +1683,14 @@
         <v>0.875</v>
       </c>
       <c r="D21" s="35"/>
-      <c r="E21" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="22"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="22" t="s">
+        <v>15</v>
+      </c>
       <c r="G21" s="29"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="43" t="s">
         <v>36</v>
       </c>
@@ -1570,15 +1700,15 @@
       <c r="C22" s="5">
         <v>0.5</v>
       </c>
-      <c r="D22" s="32" t="s">
-        <v>15</v>
-      </c>
+      <c r="D22" s="32"/>
       <c r="E22" s="17"/>
-      <c r="F22" s="18"/>
+      <c r="F22" s="18" t="s">
+        <v>15</v>
+      </c>
       <c r="G22" s="24"/>
       <c r="H22" s="46"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="44" t="s">
         <v>37</v>
       </c>
@@ -1588,15 +1718,15 @@
       <c r="C23" s="6">
         <v>0.875</v>
       </c>
-      <c r="D23" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="D23" s="33"/>
       <c r="E23" s="19"/>
-      <c r="F23" s="20"/>
+      <c r="F23" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="G23" s="23"/>
       <c r="H23" s="47"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="44" t="s">
         <v>38</v>
       </c>
@@ -1606,15 +1736,15 @@
       <c r="C24" s="6">
         <v>0.875</v>
       </c>
-      <c r="D24" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="D24" s="33"/>
       <c r="E24" s="19"/>
-      <c r="F24" s="20"/>
+      <c r="F24" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="G24" s="23"/>
       <c r="H24" s="47"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="44" t="s">
         <v>39</v>
       </c>
@@ -1624,15 +1754,15 @@
       <c r="C25" s="6">
         <v>0.875</v>
       </c>
-      <c r="D25" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="D25" s="33"/>
       <c r="E25" s="19"/>
-      <c r="F25" s="20"/>
+      <c r="F25" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="G25" s="23"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="44" t="s">
         <v>40</v>
       </c>
@@ -1643,14 +1773,14 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D26" s="33"/>
-      <c r="E26" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="20"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="G26" s="23"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="44" t="s">
         <v>41</v>
       </c>
@@ -1661,14 +1791,14 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D27" s="33"/>
-      <c r="E27" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="20"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="G27" s="23"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="44" t="s">
         <v>42</v>
       </c>
@@ -1679,14 +1809,14 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D28" s="34"/>
-      <c r="E28" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="27"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="G28" s="23"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="44" t="s">
         <v>43</v>
       </c>
@@ -1697,14 +1827,14 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="D29" s="34"/>
-      <c r="E29" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="27"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="G29" s="23"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="44" t="s">
         <v>44</v>
       </c>
@@ -1715,14 +1845,14 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="D30" s="34"/>
-      <c r="E30" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="27"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="G30" s="23"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="44" t="s">
         <v>45</v>
       </c>
@@ -1733,14 +1863,14 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="D31" s="34"/>
-      <c r="E31" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="27"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="G31" s="23"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="44" t="s">
         <v>46</v>
       </c>
@@ -1751,14 +1881,14 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="D32" s="34"/>
-      <c r="E32" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F32" s="27"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="G32" s="23"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="45" t="s">
         <v>47</v>
       </c>
@@ -1769,14 +1899,407 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D33" s="35"/>
-      <c r="E33" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" s="22"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="22" t="s">
+        <v>15</v>
+      </c>
       <c r="G33" s="29"/>
       <c r="H33" s="3"/>
     </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="8">
+        <v>41176</v>
+      </c>
+      <c r="C34" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="32"/>
+      <c r="E34" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="18"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="48"/>
+      <c r="L34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="9">
+        <v>41180</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D35" s="33"/>
+      <c r="E35" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="20"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="48"/>
+      <c r="L35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="9">
+        <v>41180</v>
+      </c>
+      <c r="C36" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D36" s="33"/>
+      <c r="E36" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="20"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
+      <c r="K36" s="48"/>
+      <c r="L36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C37" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D37" s="33"/>
+      <c r="E37" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="20"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="48"/>
+      <c r="L37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D38" s="33"/>
+      <c r="E38" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="20"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="48"/>
+      <c r="J38" s="48"/>
+      <c r="K38" s="48"/>
+      <c r="L38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D39" s="34"/>
+      <c r="E39" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="27"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
+      <c r="K39" s="48"/>
+      <c r="L39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C40" s="6">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="D40" s="34"/>
+      <c r="E40" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="27"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="48"/>
+      <c r="K40" s="48"/>
+      <c r="L40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C41" s="6">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="D41" s="34"/>
+      <c r="E41" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="27"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="48"/>
+      <c r="K41" s="48"/>
+      <c r="L41" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C42" s="6">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="D42" s="34"/>
+      <c r="E42" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="27"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
+      <c r="K42" s="48"/>
+      <c r="L42" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C43" s="6">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="D43" s="34"/>
+      <c r="E43" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="27"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="48"/>
+      <c r="L43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="42">
+        <v>41176</v>
+      </c>
+      <c r="C44" s="49">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D44" s="34"/>
+      <c r="E44" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" s="27"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="51"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="48"/>
+      <c r="K44" s="48"/>
+      <c r="L44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C45" s="6">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="D45" s="33"/>
+      <c r="E45" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" s="20"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="48"/>
+      <c r="L45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C46" s="6">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="D46" s="34"/>
+      <c r="E46" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="27"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
+      <c r="K46" s="48"/>
+      <c r="L46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C47" s="6">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="D47" s="34"/>
+      <c r="E47" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" s="27"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="48"/>
+      <c r="K47" s="48"/>
+      <c r="L47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="9">
+        <v>41176</v>
+      </c>
+      <c r="C48" s="6">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="D48" s="34"/>
+      <c r="E48" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="27"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="48"/>
+      <c r="J48" s="48"/>
+      <c r="K48" s="48"/>
+      <c r="L48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49" s="10">
+        <v>41176</v>
+      </c>
+      <c r="C49" s="7">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D49" s="35"/>
+      <c r="E49" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="22"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="48"/>
+      <c r="J49" s="48"/>
+      <c r="K49" s="48"/>
+      <c r="L49" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="I34:K49">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1788,7 +2311,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1800,7 +2323,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>